<commit_message>
Adding Walker upper and lower limits to estimates
</commit_message>
<xml_diff>
--- a/results/tables.xlsx
+++ b/results/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\3. PhD\WQE\WQE II\gmh_econ\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ACCE24-5AF9-4ACE-BAE6-CFC0BAC9465E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0022846-6480-48F1-AA9B-921AD11BE2F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="19005" windowHeight="13365" activeTab="1" xr2:uid="{09EDDA4F-F879-48C5-871F-ACF535CF1A26}"/>
+    <workbookView xWindow="8820" yWindow="2100" windowWidth="19005" windowHeight="13365" activeTab="1" xr2:uid="{09EDDA4F-F879-48C5-871F-ACF535CF1A26}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -199,12 +199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -215,6 +209,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -298,7 +298,7 @@
             <v>0.16</v>
           </cell>
           <cell r="D3">
-            <v>0.22</v>
+            <v>0.21</v>
           </cell>
         </row>
         <row r="4">
@@ -309,7 +309,7 @@
             <v>0.79</v>
           </cell>
           <cell r="D4">
-            <v>1.1200000000000001</v>
+            <v>1.06</v>
           </cell>
         </row>
         <row r="5">
@@ -320,7 +320,7 @@
             <v>1.8</v>
           </cell>
           <cell r="D5">
-            <v>2.54</v>
+            <v>2.41</v>
           </cell>
         </row>
         <row r="6">
@@ -331,7 +331,7 @@
             <v>5.4</v>
           </cell>
           <cell r="D6">
-            <v>7.63</v>
+            <v>7.23</v>
           </cell>
         </row>
       </sheetData>
@@ -344,52 +344,52 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table2_upper"/>
+      <sheetName val="table2"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3">
-            <v>0.16</v>
+            <v>0.13</v>
           </cell>
           <cell r="C3">
-            <v>0.47</v>
+            <v>0.3</v>
           </cell>
           <cell r="D3">
-            <v>0.51</v>
+            <v>0.36</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>0.82</v>
+            <v>0.63</v>
           </cell>
           <cell r="C4">
-            <v>2.34</v>
+            <v>1.5</v>
           </cell>
           <cell r="D4">
-            <v>2.5299999999999998</v>
+            <v>1.79</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>1.85</v>
+            <v>1.42</v>
           </cell>
           <cell r="C5">
-            <v>5.32</v>
+            <v>3.41</v>
           </cell>
           <cell r="D5">
-            <v>5.74</v>
+            <v>4.07</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6">
-            <v>5.55</v>
+            <v>4.2699999999999996</v>
           </cell>
           <cell r="C6">
-            <v>15.95</v>
+            <v>10.24</v>
           </cell>
           <cell r="D6">
-            <v>17.21</v>
+            <v>12.2</v>
           </cell>
         </row>
       </sheetData>
@@ -402,52 +402,52 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table2"/>
+      <sheetName val="table2_upper"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="3">
           <cell r="B3">
-            <v>0.13</v>
+            <v>0.16</v>
           </cell>
           <cell r="C3">
-            <v>0.3</v>
+            <v>0.47</v>
           </cell>
           <cell r="D3">
-            <v>0.36</v>
+            <v>0.52</v>
           </cell>
         </row>
         <row r="4">
           <cell r="B4">
-            <v>0.63</v>
+            <v>0.82</v>
           </cell>
           <cell r="C4">
-            <v>1.5</v>
+            <v>2.34</v>
           </cell>
           <cell r="D4">
-            <v>1.79</v>
+            <v>2.6</v>
           </cell>
         </row>
         <row r="5">
           <cell r="B5">
-            <v>1.42</v>
+            <v>1.85</v>
           </cell>
           <cell r="C5">
-            <v>3.41</v>
+            <v>5.32</v>
           </cell>
           <cell r="D5">
-            <v>4.07</v>
+            <v>5.91</v>
           </cell>
         </row>
         <row r="6">
           <cell r="B6">
-            <v>4.2699999999999996</v>
+            <v>5.55</v>
           </cell>
           <cell r="C6">
-            <v>10.24</v>
+            <v>15.95</v>
           </cell>
           <cell r="D6">
-            <v>12.2</v>
+            <v>17.73</v>
           </cell>
         </row>
       </sheetData>
@@ -460,104 +460,32 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_income"/>
+      <sheetName val="table1_global_lower"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
+          <cell r="C2">
+            <v>92.995000000000005</v>
+          </cell>
           <cell r="D2">
-            <v>24.52</v>
-          </cell>
-          <cell r="E2">
-            <v>6.68</v>
+            <v>4.07</v>
           </cell>
         </row>
         <row r="3">
+          <cell r="C3">
+            <v>158.57</v>
+          </cell>
           <cell r="D3">
-            <v>45.645000000000003</v>
-          </cell>
-          <cell r="E3">
-            <v>5.57</v>
+            <v>6.94</v>
           </cell>
         </row>
         <row r="4">
+          <cell r="C4">
+            <v>212.29499999999999</v>
+          </cell>
           <cell r="D4">
-            <v>44.924999999999997</v>
-          </cell>
-          <cell r="E4">
-            <v>4.28</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>10.146000000000001</v>
-          </cell>
-          <cell r="E5">
-            <v>3.36</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>66.054000000000002</v>
-          </cell>
-          <cell r="E7">
-            <v>17.989999999999998</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>110.012</v>
-          </cell>
-          <cell r="E8">
-            <v>13.43</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>105.06699999999999</v>
-          </cell>
-          <cell r="E9">
-            <v>10.02</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>19.427</v>
-          </cell>
-          <cell r="E10">
-            <v>6.44</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>66.816000000000003</v>
-          </cell>
-          <cell r="E12">
-            <v>18.2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>124.20099999999999</v>
-          </cell>
-          <cell r="E13">
-            <v>15.16</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>132.161</v>
-          </cell>
-          <cell r="E14">
-            <v>12.6</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>31.835000000000001</v>
-          </cell>
-          <cell r="E15">
-            <v>10.55</v>
+            <v>9.2899999999999991</v>
           </cell>
         </row>
       </sheetData>
@@ -570,143 +498,32 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_region"/>
+      <sheetName val="table1_global_upper"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
-          <cell r="B2" t="str">
-            <v>Europe</v>
+          <cell r="C2">
+            <v>163.178</v>
           </cell>
           <cell r="D2">
-            <v>14.439</v>
-          </cell>
-          <cell r="E2">
-            <v>5.69</v>
+            <v>5.81</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="B3" t="str">
-            <v>Asia</v>
+          <cell r="C3">
+            <v>468.55</v>
           </cell>
           <cell r="D3">
-            <v>70.012</v>
-          </cell>
-          <cell r="E3">
-            <v>5.04</v>
+            <v>16.670000000000002</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="B4" t="str">
-            <v>Oceania</v>
+          <cell r="C4">
+            <v>520.76400000000001</v>
           </cell>
           <cell r="D4">
-            <v>0.877</v>
-          </cell>
-          <cell r="E4">
-            <v>6.81</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Americas</v>
-          </cell>
-          <cell r="D5">
-            <v>20.359000000000002</v>
-          </cell>
-          <cell r="E5">
-            <v>6.68</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6" t="str">
-            <v>Africa</v>
-          </cell>
-          <cell r="D6">
-            <v>19.547999999999998</v>
-          </cell>
-          <cell r="E6">
-            <v>3.4</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>39.512999999999998</v>
-          </cell>
-          <cell r="E7">
-            <v>15.56</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>172.024</v>
-          </cell>
-          <cell r="E8">
-            <v>12.37</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>1.94</v>
-          </cell>
-          <cell r="E9">
-            <v>15.06</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>48.06</v>
-          </cell>
-          <cell r="E10">
-            <v>15.77</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>39.023000000000003</v>
-          </cell>
-          <cell r="E11">
-            <v>6.79</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>41.031999999999996</v>
-          </cell>
-          <cell r="E12">
-            <v>16.16</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>197.46899999999999</v>
-          </cell>
-          <cell r="E13">
-            <v>14.21</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>2.1619999999999999</v>
-          </cell>
-          <cell r="E14">
-            <v>16.78</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>54.113999999999997</v>
-          </cell>
-          <cell r="E15">
-            <v>17.760000000000002</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>60.235999999999997</v>
-          </cell>
-          <cell r="E16">
-            <v>10.48</v>
+            <v>18.53</v>
           </cell>
         </row>
       </sheetData>
@@ -719,32 +536,104 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_global_lower"/>
+      <sheetName val="table1_income"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
-          <cell r="C2">
-            <v>92.995000000000005</v>
-          </cell>
           <cell r="D2">
-            <v>4.07</v>
+            <v>24.52</v>
+          </cell>
+          <cell r="E2">
+            <v>6.68</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="C3">
-            <v>158.57</v>
-          </cell>
           <cell r="D3">
-            <v>6.94</v>
+            <v>45.645000000000003</v>
+          </cell>
+          <cell r="E3">
+            <v>5.57</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="C4">
-            <v>224.196</v>
-          </cell>
           <cell r="D4">
-            <v>9.81</v>
+            <v>44.924999999999997</v>
+          </cell>
+          <cell r="E4">
+            <v>4.28</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="D5">
+            <v>10.146000000000001</v>
+          </cell>
+          <cell r="E5">
+            <v>3.36</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7">
+            <v>66.054000000000002</v>
+          </cell>
+          <cell r="E7">
+            <v>17.989999999999998</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8">
+            <v>110.012</v>
+          </cell>
+          <cell r="E8">
+            <v>13.43</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9">
+            <v>105.06699999999999</v>
+          </cell>
+          <cell r="E9">
+            <v>10.02</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10">
+            <v>19.427</v>
+          </cell>
+          <cell r="E10">
+            <v>6.44</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="D12">
+            <v>66.816000000000003</v>
+          </cell>
+          <cell r="E12">
+            <v>18.2</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="D13">
+            <v>124.20099999999999</v>
+          </cell>
+          <cell r="E13">
+            <v>15.16</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14">
+            <v>132.161</v>
+          </cell>
+          <cell r="E14">
+            <v>12.6</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15">
+            <v>31.835000000000001</v>
+          </cell>
+          <cell r="E15">
+            <v>10.55</v>
           </cell>
         </row>
       </sheetData>
@@ -757,32 +646,104 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_global_upper"/>
+      <sheetName val="table1_income_lower"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
-          <cell r="C2">
-            <v>163.178</v>
-          </cell>
           <cell r="D2">
-            <v>5.81</v>
+            <v>18.146000000000001</v>
+          </cell>
+          <cell r="E2">
+            <v>5.67</v>
           </cell>
         </row>
         <row r="3">
-          <cell r="C3">
-            <v>468.55</v>
-          </cell>
           <cell r="D3">
-            <v>16.670000000000002</v>
+            <v>33.823999999999998</v>
+          </cell>
+          <cell r="E3">
+            <v>4.74</v>
           </cell>
         </row>
         <row r="4">
-          <cell r="C4">
-            <v>505.64800000000002</v>
-          </cell>
           <cell r="D4">
-            <v>17.989999999999998</v>
+            <v>33</v>
+          </cell>
+          <cell r="E4">
+            <v>3.59</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="D5">
+            <v>7.3680000000000003</v>
+          </cell>
+          <cell r="E5">
+            <v>2.85</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="D7">
+            <v>32.859000000000002</v>
+          </cell>
+          <cell r="E7">
+            <v>10.26</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="D8">
+            <v>54.555</v>
+          </cell>
+          <cell r="E8">
+            <v>7.64</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="D9">
+            <v>55.308</v>
+          </cell>
+          <cell r="E9">
+            <v>6.02</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="D10">
+            <v>10.48</v>
+          </cell>
+          <cell r="E10">
+            <v>4.05</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="D12">
+            <v>36.39</v>
+          </cell>
+          <cell r="E12">
+            <v>11.37</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="D13">
+            <v>68.236999999999995</v>
+          </cell>
+          <cell r="E13">
+            <v>9.56</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14">
+            <v>76.222999999999999</v>
+          </cell>
+          <cell r="E14">
+            <v>8.3000000000000007</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15">
+            <v>19.614000000000001</v>
+          </cell>
+          <cell r="E15">
+            <v>7.59</v>
           </cell>
         </row>
       </sheetData>
@@ -795,104 +756,104 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_income_lower"/>
+      <sheetName val="table1_income_upper"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
           <cell r="D2">
-            <v>18.146000000000001</v>
+            <v>32.036000000000001</v>
           </cell>
           <cell r="E2">
-            <v>5.67</v>
+            <v>7.63</v>
           </cell>
         </row>
         <row r="3">
           <cell r="D3">
-            <v>33.823999999999998</v>
+            <v>59.694000000000003</v>
           </cell>
           <cell r="E3">
-            <v>4.74</v>
+            <v>6.4</v>
           </cell>
         </row>
         <row r="4">
           <cell r="D4">
-            <v>33</v>
+            <v>58.929000000000002</v>
           </cell>
           <cell r="E4">
-            <v>3.59</v>
+            <v>4.93</v>
           </cell>
         </row>
         <row r="5">
           <cell r="D5">
-            <v>7.3680000000000003</v>
+            <v>13.468</v>
           </cell>
           <cell r="E5">
-            <v>2.85</v>
+            <v>3.82</v>
           </cell>
         </row>
         <row r="7">
           <cell r="D7">
-            <v>32.859000000000002</v>
+            <v>105.119</v>
           </cell>
           <cell r="E7">
-            <v>10.26</v>
+            <v>25.05</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8">
-            <v>54.555</v>
+            <v>177.09700000000001</v>
           </cell>
           <cell r="E8">
-            <v>7.64</v>
+            <v>18.98</v>
           </cell>
         </row>
         <row r="9">
           <cell r="D9">
-            <v>55.308</v>
+            <v>165.34200000000001</v>
           </cell>
           <cell r="E9">
-            <v>6.02</v>
+            <v>13.83</v>
           </cell>
         </row>
         <row r="10">
           <cell r="D10">
-            <v>10.48</v>
+            <v>30.821000000000002</v>
           </cell>
           <cell r="E10">
-            <v>4.05</v>
+            <v>8.74</v>
           </cell>
         </row>
         <row r="12">
           <cell r="D12">
-            <v>38.052</v>
+            <v>98.707999999999998</v>
           </cell>
           <cell r="E12">
-            <v>11.88</v>
+            <v>23.52</v>
           </cell>
         </row>
         <row r="13">
           <cell r="D13">
-            <v>71.590999999999994</v>
+            <v>186.78399999999999</v>
           </cell>
           <cell r="E13">
-            <v>10.029999999999999</v>
+            <v>20.02</v>
           </cell>
         </row>
         <row r="14">
           <cell r="D14">
-            <v>81.957999999999998</v>
+            <v>197.64400000000001</v>
           </cell>
           <cell r="E14">
-            <v>8.92</v>
+            <v>16.53</v>
           </cell>
         </row>
         <row r="15">
           <cell r="D15">
-            <v>21.367000000000001</v>
+            <v>47.482999999999997</v>
           </cell>
           <cell r="E15">
-            <v>8.27</v>
+            <v>13.47</v>
           </cell>
         </row>
       </sheetData>
@@ -905,104 +866,143 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_income_upper"/>
+      <sheetName val="table1_region"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
+          <cell r="B2" t="str">
+            <v>Europe</v>
+          </cell>
           <cell r="D2">
-            <v>32.036000000000001</v>
+            <v>14.439</v>
           </cell>
           <cell r="E2">
-            <v>7.63</v>
+            <v>5.69</v>
           </cell>
         </row>
         <row r="3">
+          <cell r="B3" t="str">
+            <v>Asia</v>
+          </cell>
           <cell r="D3">
-            <v>59.694000000000003</v>
+            <v>70.012</v>
           </cell>
           <cell r="E3">
-            <v>6.4</v>
+            <v>5.04</v>
           </cell>
         </row>
         <row r="4">
+          <cell r="B4" t="str">
+            <v>Oceania</v>
+          </cell>
           <cell r="D4">
-            <v>58.929000000000002</v>
+            <v>0.877</v>
           </cell>
           <cell r="E4">
-            <v>4.93</v>
+            <v>6.81</v>
           </cell>
         </row>
         <row r="5">
+          <cell r="B5" t="str">
+            <v>Americas</v>
+          </cell>
           <cell r="D5">
-            <v>13.468</v>
+            <v>20.359000000000002</v>
           </cell>
           <cell r="E5">
-            <v>3.82</v>
+            <v>6.68</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Africa</v>
+          </cell>
+          <cell r="D6">
+            <v>19.547999999999998</v>
+          </cell>
+          <cell r="E6">
+            <v>3.4</v>
           </cell>
         </row>
         <row r="7">
           <cell r="D7">
-            <v>105.119</v>
+            <v>39.512999999999998</v>
           </cell>
           <cell r="E7">
-            <v>25.05</v>
+            <v>15.56</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8">
-            <v>177.09700000000001</v>
+            <v>172.024</v>
           </cell>
           <cell r="E8">
-            <v>18.98</v>
+            <v>12.37</v>
           </cell>
         </row>
         <row r="9">
           <cell r="D9">
-            <v>165.34200000000001</v>
+            <v>1.94</v>
           </cell>
           <cell r="E9">
-            <v>13.83</v>
+            <v>15.06</v>
           </cell>
         </row>
         <row r="10">
           <cell r="D10">
-            <v>30.821000000000002</v>
+            <v>48.06</v>
           </cell>
           <cell r="E10">
-            <v>8.74</v>
+            <v>15.77</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="D11">
+            <v>39.023000000000003</v>
+          </cell>
+          <cell r="E11">
+            <v>6.79</v>
           </cell>
         </row>
         <row r="12">
           <cell r="D12">
-            <v>96.66</v>
+            <v>41.031999999999996</v>
           </cell>
           <cell r="E12">
-            <v>23.03</v>
+            <v>16.16</v>
           </cell>
         </row>
         <row r="13">
           <cell r="D13">
-            <v>182.03700000000001</v>
+            <v>197.46899999999999</v>
           </cell>
           <cell r="E13">
-            <v>19.510000000000002</v>
+            <v>14.21</v>
           </cell>
         </row>
         <row r="14">
           <cell r="D14">
-            <v>189.857</v>
+            <v>2.1619999999999999</v>
           </cell>
           <cell r="E14">
-            <v>15.87</v>
+            <v>16.78</v>
           </cell>
         </row>
         <row r="15">
           <cell r="D15">
-            <v>44.71</v>
+            <v>54.113999999999997</v>
           </cell>
           <cell r="E15">
-            <v>12.68</v>
+            <v>17.760000000000002</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="D16">
+            <v>60.235999999999997</v>
+          </cell>
+          <cell r="E16">
+            <v>10.48</v>
           </cell>
         </row>
       </sheetData>
@@ -1015,128 +1015,128 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_region_upper"/>
+      <sheetName val="table1_region_lower"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
           <cell r="D2">
-            <v>18.937000000000001</v>
+            <v>10.643000000000001</v>
           </cell>
           <cell r="E2">
-            <v>6.52</v>
+            <v>4.8</v>
           </cell>
         </row>
         <row r="3">
           <cell r="D3">
-            <v>91.448999999999998</v>
+            <v>51.761000000000003</v>
           </cell>
           <cell r="E3">
-            <v>5.79</v>
+            <v>4.25</v>
           </cell>
         </row>
         <row r="4">
           <cell r="D4">
-            <v>1.153</v>
+            <v>0.64500000000000002</v>
           </cell>
           <cell r="E4">
-            <v>7.6</v>
+            <v>5.9</v>
           </cell>
         </row>
         <row r="5">
           <cell r="D5">
-            <v>26.640999999999998</v>
+            <v>15.061</v>
           </cell>
           <cell r="E5">
-            <v>7.65</v>
+            <v>5.66</v>
           </cell>
         </row>
         <row r="6">
           <cell r="D6">
-            <v>25.948</v>
+            <v>14.228</v>
           </cell>
           <cell r="E6">
-            <v>3.89</v>
+            <v>2.87</v>
           </cell>
         </row>
         <row r="7">
           <cell r="D7">
-            <v>63.347999999999999</v>
+            <v>20.509</v>
           </cell>
           <cell r="E7">
-            <v>21.82</v>
+            <v>9.25</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8">
-            <v>273.88600000000002</v>
+            <v>87.001999999999995</v>
           </cell>
           <cell r="E8">
-            <v>17.329999999999998</v>
+            <v>7.15</v>
           </cell>
         </row>
         <row r="9">
           <cell r="D9">
-            <v>3.0329999999999999</v>
+            <v>1.028</v>
           </cell>
           <cell r="E9">
-            <v>19.98</v>
+            <v>9.4</v>
           </cell>
         </row>
         <row r="10">
           <cell r="D10">
-            <v>75.671999999999997</v>
+            <v>24.084</v>
           </cell>
           <cell r="E10">
-            <v>21.74</v>
+            <v>9.0399999999999991</v>
           </cell>
         </row>
         <row r="11">
           <cell r="D11">
-            <v>62.441000000000003</v>
+            <v>20.579000000000001</v>
           </cell>
           <cell r="E11">
-            <v>9.36</v>
+            <v>4.16</v>
           </cell>
         </row>
         <row r="12">
           <cell r="D12">
-            <v>59.427999999999997</v>
+            <v>23.170999999999999</v>
           </cell>
           <cell r="E12">
-            <v>20.47</v>
+            <v>10.45</v>
           </cell>
         </row>
         <row r="13">
           <cell r="D13">
-            <v>287.38499999999999</v>
+            <v>109.18</v>
           </cell>
           <cell r="E13">
-            <v>18.190000000000001</v>
+            <v>8.9700000000000006</v>
           </cell>
         </row>
         <row r="14">
           <cell r="D14">
-            <v>3.0950000000000002</v>
+            <v>1.242</v>
           </cell>
           <cell r="E14">
-            <v>20.399999999999999</v>
+            <v>11.36</v>
           </cell>
         </row>
         <row r="15">
           <cell r="D15">
-            <v>77.786000000000001</v>
+            <v>30.268000000000001</v>
           </cell>
           <cell r="E15">
-            <v>22.35</v>
+            <v>11.37</v>
           </cell>
         </row>
         <row r="16">
           <cell r="D16">
-            <v>85.570999999999998</v>
+            <v>36.603000000000002</v>
           </cell>
           <cell r="E16">
-            <v>12.82</v>
+            <v>7.39</v>
           </cell>
         </row>
       </sheetData>
@@ -1149,128 +1149,128 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="table1_region_lower"/>
+      <sheetName val="table1_region_upper"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="2">
           <cell r="D2">
-            <v>10.643000000000001</v>
+            <v>18.937000000000001</v>
           </cell>
           <cell r="E2">
-            <v>4.8</v>
+            <v>6.52</v>
           </cell>
         </row>
         <row r="3">
           <cell r="D3">
-            <v>51.761000000000003</v>
+            <v>91.448999999999998</v>
           </cell>
           <cell r="E3">
-            <v>4.25</v>
+            <v>5.79</v>
           </cell>
         </row>
         <row r="4">
           <cell r="D4">
-            <v>0.64500000000000002</v>
+            <v>1.153</v>
           </cell>
           <cell r="E4">
-            <v>5.9</v>
+            <v>7.6</v>
           </cell>
         </row>
         <row r="5">
           <cell r="D5">
-            <v>15.061</v>
+            <v>26.640999999999998</v>
           </cell>
           <cell r="E5">
-            <v>5.66</v>
+            <v>7.65</v>
           </cell>
         </row>
         <row r="6">
           <cell r="D6">
-            <v>14.228</v>
+            <v>25.948</v>
           </cell>
           <cell r="E6">
-            <v>2.87</v>
+            <v>3.89</v>
           </cell>
         </row>
         <row r="7">
           <cell r="D7">
-            <v>20.509</v>
+            <v>63.347999999999999</v>
           </cell>
           <cell r="E7">
-            <v>9.25</v>
+            <v>21.82</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8">
-            <v>87.001999999999995</v>
+            <v>273.88600000000002</v>
           </cell>
           <cell r="E8">
-            <v>7.15</v>
+            <v>17.329999999999998</v>
           </cell>
         </row>
         <row r="9">
           <cell r="D9">
-            <v>1.028</v>
+            <v>3.0329999999999999</v>
           </cell>
           <cell r="E9">
-            <v>9.4</v>
+            <v>19.98</v>
           </cell>
         </row>
         <row r="10">
           <cell r="D10">
-            <v>24.084</v>
+            <v>75.671999999999997</v>
           </cell>
           <cell r="E10">
-            <v>9.0399999999999991</v>
+            <v>21.74</v>
           </cell>
         </row>
         <row r="11">
           <cell r="D11">
-            <v>20.579000000000001</v>
+            <v>62.441000000000003</v>
           </cell>
           <cell r="E11">
-            <v>4.16</v>
+            <v>9.36</v>
           </cell>
         </row>
         <row r="12">
           <cell r="D12">
-            <v>24.35</v>
+            <v>60.942999999999998</v>
           </cell>
           <cell r="E12">
-            <v>10.98</v>
+            <v>20.99</v>
           </cell>
         </row>
         <row r="13">
           <cell r="D13">
-            <v>116.044</v>
+            <v>296.53699999999998</v>
           </cell>
           <cell r="E13">
-            <v>9.5399999999999991</v>
+            <v>18.77</v>
           </cell>
         </row>
         <row r="14">
           <cell r="D14">
-            <v>1.3069999999999999</v>
+            <v>3.1920000000000002</v>
           </cell>
           <cell r="E14">
-            <v>11.95</v>
+            <v>21.03</v>
           </cell>
         </row>
         <row r="15">
           <cell r="D15">
-            <v>31.754000000000001</v>
+            <v>79.807000000000002</v>
           </cell>
           <cell r="E15">
-            <v>11.93</v>
+            <v>22.93</v>
           </cell>
         </row>
         <row r="16">
           <cell r="D16">
-            <v>39.512999999999998</v>
+            <v>90.141999999999996</v>
           </cell>
           <cell r="E16">
-            <v>7.98</v>
+            <v>13.51</v>
           </cell>
         </row>
       </sheetData>
@@ -1578,8 +1578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9EF483-04C1-4FD9-B6B8-F8A403B1D01C}">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A1:X15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X15" sqref="B4:X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1587,8 +1587,8 @@
     <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="1" customWidth="1"/>
-    <col min="6" max="8" width="8.42578125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="1" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="1" style="4" customWidth="1"/>
     <col min="10" max="12" width="8.42578125" customWidth="1"/>
     <col min="13" max="13" width="1" customWidth="1"/>
     <col min="14" max="16" width="8.42578125" customWidth="1"/>
@@ -1598,127 +1598,127 @@
     <col min="22" max="24" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="6" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:24" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="5" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
     </row>
-    <row r="2" spans="1:24" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="5" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="5" t="s">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="5" t="s">
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="5" t="s">
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
     </row>
-    <row r="3" spans="1:24" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="1:24" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="P3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="R3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="T3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="V3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="W3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="X3" s="6" t="s">
+      <c r="X3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1731,23 +1731,23 @@
         <v>125.31100000000001</v>
       </c>
       <c r="C4">
-        <f>[4]table1_global_lower!$C$2</f>
+        <f>[2]table1_global_lower!$C$2</f>
         <v>92.995000000000005</v>
       </c>
       <c r="D4">
-        <f>[5]table1_global_upper!$C$2</f>
+        <f>[3]table1_global_upper!$C$2</f>
         <v>163.178</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="4">
         <f>[1]table1_global!$D$2</f>
         <v>4.9400000000000004</v>
       </c>
-      <c r="G4" s="6">
-        <f>[4]table1_global_lower!$D$2</f>
+      <c r="G4" s="4">
+        <f>[2]table1_global_lower!$D$2</f>
         <v>4.07</v>
       </c>
-      <c r="H4" s="6">
-        <f>[5]table1_global_upper!$D$2</f>
+      <c r="H4" s="4">
+        <f>[3]table1_global_upper!$D$2</f>
         <v>5.81</v>
       </c>
       <c r="J4">
@@ -1755,11 +1755,11 @@
         <v>300.72699999999998</v>
       </c>
       <c r="K4">
-        <f>[4]table1_global_lower!$C$3</f>
+        <f>[2]table1_global_lower!$C$3</f>
         <v>158.57</v>
       </c>
       <c r="L4">
-        <f>[5]table1_global_upper!$C$3</f>
+        <f>[3]table1_global_upper!$C$3</f>
         <v>468.55</v>
       </c>
       <c r="N4">
@@ -1767,11 +1767,11 @@
         <v>11.85</v>
       </c>
       <c r="O4">
-        <f>[4]table1_global_lower!$D$3</f>
+        <f>[2]table1_global_lower!$D$3</f>
         <v>6.94</v>
       </c>
       <c r="P4">
-        <f>[5]table1_global_upper!$D$3</f>
+        <f>[3]table1_global_upper!$D$3</f>
         <v>16.670000000000002</v>
       </c>
       <c r="R4">
@@ -1779,24 +1779,24 @@
         <v>358.46600000000001</v>
       </c>
       <c r="S4">
-        <f>[4]table1_global_lower!$C$4</f>
-        <v>224.196</v>
+        <f>[2]table1_global_lower!$C$4</f>
+        <v>212.29499999999999</v>
       </c>
       <c r="T4">
-        <f>[5]table1_global_upper!$C$4</f>
-        <v>505.64800000000002</v>
+        <f>[3]table1_global_upper!$C$4</f>
+        <v>520.76400000000001</v>
       </c>
       <c r="V4">
         <f>[1]table1_global!$D$4</f>
         <v>14.12</v>
       </c>
       <c r="W4">
-        <f>[4]table1_global_lower!$D$4</f>
-        <v>9.81</v>
+        <f>[2]table1_global_lower!$D$4</f>
+        <v>9.2899999999999991</v>
       </c>
       <c r="X4">
-        <f>[5]table1_global_upper!$D$4</f>
-        <v>17.989999999999998</v>
+        <f>[3]table1_global_upper!$D$4</f>
+        <v>18.53</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -1804,76 +1804,76 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <f>[2]table1_income!D2</f>
+        <f>[4]table1_income!D2</f>
         <v>24.52</v>
       </c>
       <c r="C6">
-        <f>[6]table1_income_lower!D2</f>
+        <f>[5]table1_income_lower!D2</f>
         <v>18.146000000000001</v>
       </c>
       <c r="D6">
-        <f>[7]table1_income_upper!D2</f>
+        <f>[6]table1_income_upper!D2</f>
         <v>32.036000000000001</v>
       </c>
-      <c r="F6" s="6">
-        <f>[2]table1_income!E2</f>
+      <c r="F6" s="4">
+        <f>[4]table1_income!E2</f>
         <v>6.68</v>
       </c>
-      <c r="G6" s="6">
-        <f>[6]table1_income_lower!E2</f>
+      <c r="G6" s="4">
+        <f>[5]table1_income_lower!E2</f>
         <v>5.67</v>
       </c>
-      <c r="H6" s="6">
-        <f>[7]table1_income_upper!E2</f>
+      <c r="H6" s="4">
+        <f>[6]table1_income_upper!E2</f>
         <v>7.63</v>
       </c>
       <c r="J6">
-        <f>[2]table1_income!D7</f>
+        <f>[4]table1_income!D7</f>
         <v>66.054000000000002</v>
       </c>
       <c r="K6">
-        <f>[6]table1_income_lower!D7</f>
+        <f>[5]table1_income_lower!D7</f>
         <v>32.859000000000002</v>
       </c>
       <c r="L6">
-        <f>[7]table1_income_upper!D7</f>
+        <f>[6]table1_income_upper!D7</f>
         <v>105.119</v>
       </c>
       <c r="N6">
-        <f>[2]table1_income!E7</f>
+        <f>[4]table1_income!E7</f>
         <v>17.989999999999998</v>
       </c>
       <c r="O6">
-        <f>[6]table1_income_lower!E7</f>
+        <f>[5]table1_income_lower!E7</f>
         <v>10.26</v>
       </c>
       <c r="P6">
-        <f>[7]table1_income_upper!E7</f>
+        <f>[6]table1_income_upper!E7</f>
         <v>25.05</v>
       </c>
       <c r="R6">
-        <f>[2]table1_income!D12</f>
+        <f>[4]table1_income!D12</f>
         <v>66.816000000000003</v>
       </c>
       <c r="S6">
-        <f>[6]table1_income_lower!D12</f>
-        <v>38.052</v>
+        <f>[5]table1_income_lower!D12</f>
+        <v>36.39</v>
       </c>
       <c r="T6">
-        <f>[7]table1_income_upper!D12</f>
-        <v>96.66</v>
+        <f>[6]table1_income_upper!D12</f>
+        <v>98.707999999999998</v>
       </c>
       <c r="V6">
-        <f>[2]table1_income!E12</f>
+        <f>[4]table1_income!E12</f>
         <v>18.2</v>
       </c>
       <c r="W6">
-        <f>[6]table1_income_lower!E12</f>
-        <v>11.88</v>
+        <f>[5]table1_income_lower!E12</f>
+        <v>11.37</v>
       </c>
       <c r="X6">
-        <f>[7]table1_income_upper!E12</f>
-        <v>23.03</v>
+        <f>[6]table1_income_upper!E12</f>
+        <v>23.52</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -1881,76 +1881,76 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f>[2]table1_income!D3</f>
+        <f>[4]table1_income!D3</f>
         <v>45.645000000000003</v>
       </c>
       <c r="C7">
-        <f>[6]table1_income_lower!D3</f>
+        <f>[5]table1_income_lower!D3</f>
         <v>33.823999999999998</v>
       </c>
       <c r="D7">
-        <f>[7]table1_income_upper!D3</f>
+        <f>[6]table1_income_upper!D3</f>
         <v>59.694000000000003</v>
       </c>
-      <c r="F7" s="6">
-        <f>[2]table1_income!E3</f>
+      <c r="F7" s="4">
+        <f>[4]table1_income!E3</f>
         <v>5.57</v>
       </c>
-      <c r="G7" s="6">
-        <f>[6]table1_income_lower!E3</f>
+      <c r="G7" s="4">
+        <f>[5]table1_income_lower!E3</f>
         <v>4.74</v>
       </c>
-      <c r="H7" s="6">
-        <f>[7]table1_income_upper!E3</f>
+      <c r="H7" s="4">
+        <f>[6]table1_income_upper!E3</f>
         <v>6.4</v>
       </c>
       <c r="J7">
-        <f>[2]table1_income!D8</f>
+        <f>[4]table1_income!D8</f>
         <v>110.012</v>
       </c>
       <c r="K7">
-        <f>[6]table1_income_lower!D8</f>
+        <f>[5]table1_income_lower!D8</f>
         <v>54.555</v>
       </c>
       <c r="L7">
-        <f>[7]table1_income_upper!D8</f>
+        <f>[6]table1_income_upper!D8</f>
         <v>177.09700000000001</v>
       </c>
       <c r="N7">
-        <f>[2]table1_income!E8</f>
+        <f>[4]table1_income!E8</f>
         <v>13.43</v>
       </c>
       <c r="O7">
-        <f>[6]table1_income_lower!E8</f>
+        <f>[5]table1_income_lower!E8</f>
         <v>7.64</v>
       </c>
       <c r="P7">
-        <f>[7]table1_income_upper!E8</f>
+        <f>[6]table1_income_upper!E8</f>
         <v>18.98</v>
       </c>
       <c r="R7">
-        <f>[2]table1_income!D13</f>
+        <f>[4]table1_income!D13</f>
         <v>124.20099999999999</v>
       </c>
       <c r="S7">
-        <f>[6]table1_income_lower!D13</f>
-        <v>71.590999999999994</v>
+        <f>[5]table1_income_lower!D13</f>
+        <v>68.236999999999995</v>
       </c>
       <c r="T7">
-        <f>[7]table1_income_upper!D13</f>
-        <v>182.03700000000001</v>
+        <f>[6]table1_income_upper!D13</f>
+        <v>186.78399999999999</v>
       </c>
       <c r="V7">
-        <f>[2]table1_income!E13</f>
+        <f>[4]table1_income!E13</f>
         <v>15.16</v>
       </c>
       <c r="W7">
-        <f>[6]table1_income_lower!E13</f>
-        <v>10.029999999999999</v>
+        <f>[5]table1_income_lower!E13</f>
+        <v>9.56</v>
       </c>
       <c r="X7">
-        <f>[7]table1_income_upper!E13</f>
-        <v>19.510000000000002</v>
+        <f>[6]table1_income_upper!E13</f>
+        <v>20.02</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1958,76 +1958,76 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f>[2]table1_income!D4</f>
+        <f>[4]table1_income!D4</f>
         <v>44.924999999999997</v>
       </c>
       <c r="C8">
-        <f>[6]table1_income_lower!D4</f>
+        <f>[5]table1_income_lower!D4</f>
         <v>33</v>
       </c>
       <c r="D8">
-        <f>[7]table1_income_upper!D4</f>
+        <f>[6]table1_income_upper!D4</f>
         <v>58.929000000000002</v>
       </c>
-      <c r="F8" s="6">
-        <f>[2]table1_income!E4</f>
+      <c r="F8" s="4">
+        <f>[4]table1_income!E4</f>
         <v>4.28</v>
       </c>
-      <c r="G8" s="6">
-        <f>[6]table1_income_lower!E4</f>
+      <c r="G8" s="4">
+        <f>[5]table1_income_lower!E4</f>
         <v>3.59</v>
       </c>
-      <c r="H8" s="6">
-        <f>[7]table1_income_upper!E4</f>
+      <c r="H8" s="4">
+        <f>[6]table1_income_upper!E4</f>
         <v>4.93</v>
       </c>
       <c r="J8">
-        <f>[2]table1_income!D9</f>
+        <f>[4]table1_income!D9</f>
         <v>105.06699999999999</v>
       </c>
       <c r="K8">
-        <f>[6]table1_income_lower!D9</f>
+        <f>[5]table1_income_lower!D9</f>
         <v>55.308</v>
       </c>
       <c r="L8">
-        <f>[7]table1_income_upper!D9</f>
+        <f>[6]table1_income_upper!D9</f>
         <v>165.34200000000001</v>
       </c>
       <c r="N8">
-        <f>[2]table1_income!E9</f>
+        <f>[4]table1_income!E9</f>
         <v>10.02</v>
       </c>
       <c r="O8">
-        <f>[6]table1_income_lower!E9</f>
+        <f>[5]table1_income_lower!E9</f>
         <v>6.02</v>
       </c>
       <c r="P8">
-        <f>[7]table1_income_upper!E9</f>
+        <f>[6]table1_income_upper!E9</f>
         <v>13.83</v>
       </c>
       <c r="R8">
-        <f>[2]table1_income!D14</f>
+        <f>[4]table1_income!D14</f>
         <v>132.161</v>
       </c>
       <c r="S8">
-        <f>[6]table1_income_lower!D14</f>
-        <v>81.957999999999998</v>
+        <f>[5]table1_income_lower!D14</f>
+        <v>76.222999999999999</v>
       </c>
       <c r="T8">
-        <f>[7]table1_income_upper!D14</f>
-        <v>189.857</v>
+        <f>[6]table1_income_upper!D14</f>
+        <v>197.64400000000001</v>
       </c>
       <c r="V8">
-        <f>[2]table1_income!E14</f>
+        <f>[4]table1_income!E14</f>
         <v>12.6</v>
       </c>
       <c r="W8">
-        <f>[6]table1_income_lower!E14</f>
-        <v>8.92</v>
+        <f>[5]table1_income_lower!E14</f>
+        <v>8.3000000000000007</v>
       </c>
       <c r="X8">
-        <f>[7]table1_income_upper!E14</f>
-        <v>15.87</v>
+        <f>[6]table1_income_upper!E14</f>
+        <v>16.53</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -2035,76 +2035,76 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f>[2]table1_income!D5</f>
+        <f>[4]table1_income!D5</f>
         <v>10.146000000000001</v>
       </c>
       <c r="C9">
-        <f>[6]table1_income_lower!D5</f>
+        <f>[5]table1_income_lower!D5</f>
         <v>7.3680000000000003</v>
       </c>
       <c r="D9">
-        <f>[7]table1_income_upper!D5</f>
+        <f>[6]table1_income_upper!D5</f>
         <v>13.468</v>
       </c>
-      <c r="F9" s="6">
-        <f>[2]table1_income!E5</f>
+      <c r="F9" s="4">
+        <f>[4]table1_income!E5</f>
         <v>3.36</v>
       </c>
-      <c r="G9" s="6">
-        <f>[6]table1_income_lower!E5</f>
+      <c r="G9" s="4">
+        <f>[5]table1_income_lower!E5</f>
         <v>2.85</v>
       </c>
-      <c r="H9" s="6">
-        <f>[7]table1_income_upper!E5</f>
+      <c r="H9" s="4">
+        <f>[6]table1_income_upper!E5</f>
         <v>3.82</v>
       </c>
       <c r="J9">
-        <f>[2]table1_income!D10</f>
+        <f>[4]table1_income!D10</f>
         <v>19.427</v>
       </c>
       <c r="K9">
-        <f>[6]table1_income_lower!D10</f>
+        <f>[5]table1_income_lower!D10</f>
         <v>10.48</v>
       </c>
       <c r="L9">
-        <f>[7]table1_income_upper!D10</f>
+        <f>[6]table1_income_upper!D10</f>
         <v>30.821000000000002</v>
       </c>
       <c r="N9">
-        <f>[2]table1_income!E10</f>
+        <f>[4]table1_income!E10</f>
         <v>6.44</v>
       </c>
       <c r="O9">
-        <f>[6]table1_income_lower!E10</f>
+        <f>[5]table1_income_lower!E10</f>
         <v>4.05</v>
       </c>
       <c r="P9">
-        <f>[7]table1_income_upper!E10</f>
+        <f>[6]table1_income_upper!E10</f>
         <v>8.74</v>
       </c>
       <c r="R9">
-        <f>[2]table1_income!D15</f>
+        <f>[4]table1_income!D15</f>
         <v>31.835000000000001</v>
       </c>
       <c r="S9">
-        <f>[6]table1_income_lower!D15</f>
-        <v>21.367000000000001</v>
+        <f>[5]table1_income_lower!D15</f>
+        <v>19.614000000000001</v>
       </c>
       <c r="T9">
-        <f>[7]table1_income_upper!D15</f>
-        <v>44.71</v>
+        <f>[6]table1_income_upper!D15</f>
+        <v>47.482999999999997</v>
       </c>
       <c r="V9">
-        <f>[2]table1_income!E15</f>
+        <f>[4]table1_income!E15</f>
         <v>10.55</v>
       </c>
       <c r="W9">
-        <f>[6]table1_income_lower!E15</f>
-        <v>8.27</v>
+        <f>[5]table1_income_lower!E15</f>
+        <v>7.59</v>
       </c>
       <c r="X9">
-        <f>[7]table1_income_upper!E15</f>
-        <v>12.68</v>
+        <f>[6]table1_income_upper!E15</f>
+        <v>13.47</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -2112,405 +2112,405 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>[3]table1_region!B2</f>
+        <f>[7]table1_region!B2</f>
         <v>Europe</v>
       </c>
       <c r="B11">
-        <f>[3]table1_region!D2</f>
+        <f>[7]table1_region!D2</f>
         <v>14.439</v>
       </c>
       <c r="C11">
-        <f>[9]table1_region_lower!D2</f>
+        <f>[8]table1_region_lower!D2</f>
         <v>10.643000000000001</v>
       </c>
       <c r="D11">
-        <f>[8]table1_region_upper!D2</f>
+        <f>[9]table1_region_upper!D2</f>
         <v>18.937000000000001</v>
       </c>
-      <c r="F11" s="6">
-        <f>[3]table1_region!E2</f>
+      <c r="F11" s="4">
+        <f>[7]table1_region!E2</f>
         <v>5.69</v>
       </c>
-      <c r="G11" s="6">
-        <f>[9]table1_region_lower!E2</f>
+      <c r="G11" s="4">
+        <f>[8]table1_region_lower!E2</f>
         <v>4.8</v>
       </c>
-      <c r="H11" s="6">
-        <f>[8]table1_region_upper!E2</f>
+      <c r="H11" s="4">
+        <f>[9]table1_region_upper!E2</f>
         <v>6.52</v>
       </c>
       <c r="J11">
-        <f>[3]table1_region!D7</f>
+        <f>[7]table1_region!D7</f>
         <v>39.512999999999998</v>
       </c>
-      <c r="K11" s="6">
-        <f>[9]table1_region_lower!D7</f>
+      <c r="K11" s="4">
+        <f>[8]table1_region_lower!D7</f>
         <v>20.509</v>
       </c>
       <c r="L11">
-        <f>[8]table1_region_upper!D7</f>
+        <f>[9]table1_region_upper!D7</f>
         <v>63.347999999999999</v>
       </c>
       <c r="N11">
-        <f>[3]table1_region!E7</f>
+        <f>[7]table1_region!E7</f>
         <v>15.56</v>
       </c>
       <c r="O11">
-        <f>[9]table1_region_lower!E7</f>
+        <f>[8]table1_region_lower!E7</f>
         <v>9.25</v>
       </c>
       <c r="P11">
-        <f>[8]table1_region_upper!E7</f>
+        <f>[9]table1_region_upper!E7</f>
         <v>21.82</v>
       </c>
       <c r="R11">
-        <f>[3]table1_region!D12</f>
+        <f>[7]table1_region!D12</f>
         <v>41.031999999999996</v>
       </c>
       <c r="S11">
-        <f>[9]table1_region_lower!D12</f>
-        <v>24.35</v>
+        <f>[8]table1_region_lower!D12</f>
+        <v>23.170999999999999</v>
       </c>
       <c r="T11">
-        <f>[8]table1_region_upper!D12</f>
-        <v>59.427999999999997</v>
+        <f>[9]table1_region_upper!D12</f>
+        <v>60.942999999999998</v>
       </c>
       <c r="V11">
-        <f>[3]table1_region!E12</f>
+        <f>[7]table1_region!E12</f>
         <v>16.16</v>
       </c>
       <c r="W11">
-        <f>[9]table1_region_lower!E12</f>
-        <v>10.98</v>
+        <f>[8]table1_region_lower!E12</f>
+        <v>10.45</v>
       </c>
       <c r="X11">
-        <f>[8]table1_region_upper!E12</f>
-        <v>20.47</v>
+        <f>[9]table1_region_upper!E12</f>
+        <v>20.99</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>[3]table1_region!B3</f>
+        <f>[7]table1_region!B3</f>
         <v>Asia</v>
       </c>
       <c r="B12">
-        <f>[3]table1_region!D3</f>
+        <f>[7]table1_region!D3</f>
         <v>70.012</v>
       </c>
       <c r="C12">
-        <f>[9]table1_region_lower!D3</f>
+        <f>[8]table1_region_lower!D3</f>
         <v>51.761000000000003</v>
       </c>
       <c r="D12">
-        <f>[8]table1_region_upper!D3</f>
+        <f>[9]table1_region_upper!D3</f>
         <v>91.448999999999998</v>
       </c>
-      <c r="F12" s="6">
-        <f>[3]table1_region!E3</f>
+      <c r="F12" s="4">
+        <f>[7]table1_region!E3</f>
         <v>5.04</v>
       </c>
-      <c r="G12" s="6">
-        <f>[9]table1_region_lower!E3</f>
+      <c r="G12" s="4">
+        <f>[8]table1_region_lower!E3</f>
         <v>4.25</v>
       </c>
-      <c r="H12" s="6">
-        <f>[8]table1_region_upper!E3</f>
+      <c r="H12" s="4">
+        <f>[9]table1_region_upper!E3</f>
         <v>5.79</v>
       </c>
       <c r="J12">
-        <f>[3]table1_region!D8</f>
+        <f>[7]table1_region!D8</f>
         <v>172.024</v>
       </c>
-      <c r="K12" s="6">
-        <f>[9]table1_region_lower!D8</f>
+      <c r="K12" s="4">
+        <f>[8]table1_region_lower!D8</f>
         <v>87.001999999999995</v>
       </c>
       <c r="L12">
-        <f>[8]table1_region_upper!D8</f>
+        <f>[9]table1_region_upper!D8</f>
         <v>273.88600000000002</v>
       </c>
       <c r="N12">
-        <f>[3]table1_region!E8</f>
+        <f>[7]table1_region!E8</f>
         <v>12.37</v>
       </c>
       <c r="O12">
-        <f>[9]table1_region_lower!E8</f>
+        <f>[8]table1_region_lower!E8</f>
         <v>7.15</v>
       </c>
       <c r="P12">
-        <f>[8]table1_region_upper!E8</f>
+        <f>[9]table1_region_upper!E8</f>
         <v>17.329999999999998</v>
       </c>
       <c r="R12">
-        <f>[3]table1_region!D13</f>
+        <f>[7]table1_region!D13</f>
         <v>197.46899999999999</v>
       </c>
       <c r="S12">
-        <f>[9]table1_region_lower!D13</f>
-        <v>116.044</v>
+        <f>[8]table1_region_lower!D13</f>
+        <v>109.18</v>
       </c>
       <c r="T12">
-        <f>[8]table1_region_upper!D13</f>
-        <v>287.38499999999999</v>
+        <f>[9]table1_region_upper!D13</f>
+        <v>296.53699999999998</v>
       </c>
       <c r="V12">
-        <f>[3]table1_region!E13</f>
+        <f>[7]table1_region!E13</f>
         <v>14.21</v>
       </c>
       <c r="W12">
-        <f>[9]table1_region_lower!E13</f>
-        <v>9.5399999999999991</v>
+        <f>[8]table1_region_lower!E13</f>
+        <v>8.9700000000000006</v>
       </c>
       <c r="X12">
-        <f>[8]table1_region_upper!E13</f>
-        <v>18.190000000000001</v>
+        <f>[9]table1_region_upper!E13</f>
+        <v>18.77</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>[3]table1_region!B4</f>
+        <f>[7]table1_region!B4</f>
         <v>Oceania</v>
       </c>
       <c r="B13">
-        <f>[3]table1_region!D4</f>
+        <f>[7]table1_region!D4</f>
         <v>0.877</v>
       </c>
       <c r="C13">
-        <f>[9]table1_region_lower!D4</f>
+        <f>[8]table1_region_lower!D4</f>
         <v>0.64500000000000002</v>
       </c>
       <c r="D13">
-        <f>[8]table1_region_upper!D4</f>
+        <f>[9]table1_region_upper!D4</f>
         <v>1.153</v>
       </c>
-      <c r="F13" s="6">
-        <f>[3]table1_region!E4</f>
+      <c r="F13" s="4">
+        <f>[7]table1_region!E4</f>
         <v>6.81</v>
       </c>
-      <c r="G13" s="6">
-        <f>[9]table1_region_lower!E4</f>
+      <c r="G13" s="4">
+        <f>[8]table1_region_lower!E4</f>
         <v>5.9</v>
       </c>
-      <c r="H13" s="6">
-        <f>[8]table1_region_upper!E4</f>
+      <c r="H13" s="4">
+        <f>[9]table1_region_upper!E4</f>
         <v>7.6</v>
       </c>
       <c r="J13">
-        <f>[3]table1_region!D9</f>
+        <f>[7]table1_region!D9</f>
         <v>1.94</v>
       </c>
-      <c r="K13" s="6">
-        <f>[9]table1_region_lower!D9</f>
+      <c r="K13" s="4">
+        <f>[8]table1_region_lower!D9</f>
         <v>1.028</v>
       </c>
       <c r="L13">
-        <f>[8]table1_region_upper!D9</f>
+        <f>[9]table1_region_upper!D9</f>
         <v>3.0329999999999999</v>
       </c>
       <c r="N13">
-        <f>[3]table1_region!E9</f>
+        <f>[7]table1_region!E9</f>
         <v>15.06</v>
       </c>
       <c r="O13">
-        <f>[9]table1_region_lower!E9</f>
+        <f>[8]table1_region_lower!E9</f>
         <v>9.4</v>
       </c>
       <c r="P13">
-        <f>[8]table1_region_upper!E9</f>
+        <f>[9]table1_region_upper!E9</f>
         <v>19.98</v>
       </c>
       <c r="R13">
-        <f>[3]table1_region!D14</f>
+        <f>[7]table1_region!D14</f>
         <v>2.1619999999999999</v>
       </c>
       <c r="S13">
-        <f>[9]table1_region_lower!D14</f>
-        <v>1.3069999999999999</v>
+        <f>[8]table1_region_lower!D14</f>
+        <v>1.242</v>
       </c>
       <c r="T13">
-        <f>[8]table1_region_upper!D14</f>
-        <v>3.0950000000000002</v>
+        <f>[9]table1_region_upper!D14</f>
+        <v>3.1920000000000002</v>
       </c>
       <c r="V13">
-        <f>[3]table1_region!E14</f>
+        <f>[7]table1_region!E14</f>
         <v>16.78</v>
       </c>
       <c r="W13">
-        <f>[9]table1_region_lower!E14</f>
-        <v>11.95</v>
+        <f>[8]table1_region_lower!E14</f>
+        <v>11.36</v>
       </c>
       <c r="X13">
-        <f>[8]table1_region_upper!E14</f>
-        <v>20.399999999999999</v>
+        <f>[9]table1_region_upper!E14</f>
+        <v>21.03</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>[3]table1_region!B5</f>
+        <f>[7]table1_region!B5</f>
         <v>Americas</v>
       </c>
       <c r="B14">
-        <f>[3]table1_region!D5</f>
+        <f>[7]table1_region!D5</f>
         <v>20.359000000000002</v>
       </c>
       <c r="C14">
-        <f>[9]table1_region_lower!D5</f>
+        <f>[8]table1_region_lower!D5</f>
         <v>15.061</v>
       </c>
       <c r="D14">
-        <f>[8]table1_region_upper!D5</f>
+        <f>[9]table1_region_upper!D5</f>
         <v>26.640999999999998</v>
       </c>
-      <c r="F14" s="6">
-        <f>[3]table1_region!E5</f>
+      <c r="F14" s="4">
+        <f>[7]table1_region!E5</f>
         <v>6.68</v>
       </c>
-      <c r="G14" s="6">
-        <f>[9]table1_region_lower!E5</f>
+      <c r="G14" s="4">
+        <f>[8]table1_region_lower!E5</f>
         <v>5.66</v>
       </c>
-      <c r="H14" s="6">
-        <f>[8]table1_region_upper!E5</f>
+      <c r="H14" s="4">
+        <f>[9]table1_region_upper!E5</f>
         <v>7.65</v>
       </c>
       <c r="J14">
-        <f>[3]table1_region!D10</f>
+        <f>[7]table1_region!D10</f>
         <v>48.06</v>
       </c>
-      <c r="K14" s="6">
-        <f>[9]table1_region_lower!D10</f>
+      <c r="K14" s="4">
+        <f>[8]table1_region_lower!D10</f>
         <v>24.084</v>
       </c>
       <c r="L14">
-        <f>[8]table1_region_upper!D10</f>
+        <f>[9]table1_region_upper!D10</f>
         <v>75.671999999999997</v>
       </c>
       <c r="N14">
-        <f>[3]table1_region!E10</f>
+        <f>[7]table1_region!E10</f>
         <v>15.77</v>
       </c>
       <c r="O14">
-        <f>[9]table1_region_lower!E10</f>
+        <f>[8]table1_region_lower!E10</f>
         <v>9.0399999999999991</v>
       </c>
       <c r="P14">
-        <f>[8]table1_region_upper!E10</f>
+        <f>[9]table1_region_upper!E10</f>
         <v>21.74</v>
       </c>
       <c r="R14">
-        <f>[3]table1_region!D15</f>
+        <f>[7]table1_region!D15</f>
         <v>54.113999999999997</v>
       </c>
       <c r="S14">
-        <f>[9]table1_region_lower!D15</f>
-        <v>31.754000000000001</v>
+        <f>[8]table1_region_lower!D15</f>
+        <v>30.268000000000001</v>
       </c>
       <c r="T14">
-        <f>[8]table1_region_upper!D15</f>
-        <v>77.786000000000001</v>
+        <f>[9]table1_region_upper!D15</f>
+        <v>79.807000000000002</v>
       </c>
       <c r="V14">
-        <f>[3]table1_region!E15</f>
+        <f>[7]table1_region!E15</f>
         <v>17.760000000000002</v>
       </c>
       <c r="W14">
-        <f>[9]table1_region_lower!E15</f>
-        <v>11.93</v>
+        <f>[8]table1_region_lower!E15</f>
+        <v>11.37</v>
       </c>
       <c r="X14">
-        <f>[8]table1_region_upper!E15</f>
-        <v>22.35</v>
+        <f>[9]table1_region_upper!E15</f>
+        <v>22.93</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>[3]table1_region!B6</f>
+        <f>[7]table1_region!B6</f>
         <v>Africa</v>
       </c>
       <c r="B15">
-        <f>[3]table1_region!D6</f>
+        <f>[7]table1_region!D6</f>
         <v>19.547999999999998</v>
       </c>
       <c r="C15">
-        <f>[9]table1_region_lower!D6</f>
+        <f>[8]table1_region_lower!D6</f>
         <v>14.228</v>
       </c>
       <c r="D15">
-        <f>[8]table1_region_upper!D6</f>
+        <f>[9]table1_region_upper!D6</f>
         <v>25.948</v>
       </c>
-      <c r="F15" s="6">
-        <f>[3]table1_region!E6</f>
+      <c r="F15" s="4">
+        <f>[7]table1_region!E6</f>
         <v>3.4</v>
       </c>
-      <c r="G15" s="6">
-        <f>[9]table1_region_lower!E6</f>
+      <c r="G15" s="4">
+        <f>[8]table1_region_lower!E6</f>
         <v>2.87</v>
       </c>
-      <c r="H15" s="6">
-        <f>[8]table1_region_upper!E6</f>
+      <c r="H15" s="4">
+        <f>[9]table1_region_upper!E6</f>
         <v>3.89</v>
       </c>
       <c r="J15">
-        <f>[3]table1_region!D11</f>
+        <f>[7]table1_region!D11</f>
         <v>39.023000000000003</v>
       </c>
-      <c r="K15" s="6">
-        <f>[9]table1_region_lower!D11</f>
+      <c r="K15" s="4">
+        <f>[8]table1_region_lower!D11</f>
         <v>20.579000000000001</v>
       </c>
       <c r="L15">
-        <f>[8]table1_region_upper!D11</f>
+        <f>[9]table1_region_upper!D11</f>
         <v>62.441000000000003</v>
       </c>
       <c r="N15">
-        <f>[3]table1_region!E11</f>
+        <f>[7]table1_region!E11</f>
         <v>6.79</v>
       </c>
       <c r="O15">
-        <f>[9]table1_region_lower!E11</f>
+        <f>[8]table1_region_lower!E11</f>
         <v>4.16</v>
       </c>
       <c r="P15">
-        <f>[8]table1_region_upper!E11</f>
+        <f>[9]table1_region_upper!E11</f>
         <v>9.36</v>
       </c>
       <c r="R15">
-        <f>[3]table1_region!D16</f>
+        <f>[7]table1_region!D16</f>
         <v>60.235999999999997</v>
       </c>
       <c r="S15">
-        <f>[9]table1_region_lower!D16</f>
-        <v>39.512999999999998</v>
+        <f>[8]table1_region_lower!D16</f>
+        <v>36.603000000000002</v>
       </c>
       <c r="T15">
-        <f>[8]table1_region_upper!D16</f>
-        <v>85.570999999999998</v>
+        <f>[9]table1_region_upper!D16</f>
+        <v>90.141999999999996</v>
       </c>
       <c r="V15">
-        <f>[3]table1_region!E16</f>
+        <f>[7]table1_region!E16</f>
         <v>10.48</v>
       </c>
       <c r="W15">
-        <f>[9]table1_region_lower!E16</f>
-        <v>7.98</v>
+        <f>[8]table1_region_lower!E16</f>
+        <v>7.39</v>
       </c>
       <c r="X15">
-        <f>[8]table1_region_upper!E16</f>
-        <v>12.82</v>
+        <f>[9]table1_region_upper!E16</f>
+        <v>13.51</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="V2:X2"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="B1:H1"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="N2:P2"/>
-    <mergeCell ref="V2:X2"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -2522,7 +2522,7 @@
   <dimension ref="A2:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="A2:L7"/>
+      <selection activeCell="L7" sqref="B4:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,232 +2533,232 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="3" t="str">
+      <c r="A2" s="5"/>
+      <c r="B2" s="8" t="str">
         <f>[10]table2_lower!B2</f>
         <v>Original GBD method</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="3" t="str">
+      <c r="F2" s="8" t="str">
         <f>[10]table2_lower!C2</f>
         <v>Revised - Vigo et al. method</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="3" t="str">
+      <c r="J2" s="8" t="str">
         <f>[10]table2_lower!D2</f>
         <v>Revised - Composite method</v>
       </c>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7">
-        <f>[12]table2!B3</f>
+      <c r="B4" s="5">
+        <f>[11]table2!B3</f>
         <v>0.13</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <f>[10]table2_lower!B3</f>
         <v>0.09</v>
       </c>
-      <c r="D4" s="7">
-        <f>[11]table2_upper!$B3</f>
+      <c r="D4" s="5">
+        <f>[12]table2_upper!$B3</f>
         <v>0.16</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7">
-        <f>[12]table2!C3</f>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
+        <f>[11]table2!C3</f>
         <v>0.3</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="5">
         <f>[10]table2_lower!C3</f>
         <v>0.16</v>
       </c>
-      <c r="H4" s="7">
-        <f>[11]table2_upper!$C3</f>
+      <c r="H4" s="5">
+        <f>[12]table2_upper!$C3</f>
         <v>0.47</v>
       </c>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7">
-        <f>[12]table2!D3</f>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <f>[11]table2!D3</f>
         <v>0.36</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="5">
         <f>[10]table2_lower!D3</f>
-        <v>0.22</v>
-      </c>
-      <c r="L4" s="7">
-        <f>[11]table2_upper!$D3</f>
-        <v>0.51</v>
+        <v>0.21</v>
+      </c>
+      <c r="L4" s="5">
+        <f>[12]table2_upper!$D3</f>
+        <v>0.52</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="7">
-        <f>[12]table2!B4</f>
+      <c r="B5" s="5">
+        <f>[11]table2!B4</f>
         <v>0.63</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <f>[10]table2_lower!B4</f>
         <v>0.46</v>
       </c>
-      <c r="D5" s="7">
-        <f>[11]table2_upper!$B4</f>
+      <c r="D5" s="5">
+        <f>[12]table2_upper!$B4</f>
         <v>0.82</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7">
-        <f>[12]table2!C4</f>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <f>[11]table2!C4</f>
         <v>1.5</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="5">
         <f>[10]table2_lower!C4</f>
         <v>0.79</v>
       </c>
-      <c r="H5" s="7">
-        <f>[11]table2_upper!$C4</f>
+      <c r="H5" s="5">
+        <f>[12]table2_upper!$C4</f>
         <v>2.34</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7">
-        <f>[12]table2!D4</f>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
+        <f>[11]table2!D4</f>
         <v>1.79</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="5">
         <f>[10]table2_lower!D4</f>
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="L5" s="7">
-        <f>[11]table2_upper!$D4</f>
-        <v>2.5299999999999998</v>
+        <v>1.06</v>
+      </c>
+      <c r="L5" s="5">
+        <f>[12]table2_upper!$D4</f>
+        <v>2.6</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7">
-        <f>[12]table2!B5</f>
+      <c r="B6" s="5">
+        <f>[11]table2!B5</f>
         <v>1.42</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <f>[10]table2_lower!B5</f>
         <v>1.06</v>
       </c>
-      <c r="D6" s="7">
-        <f>[11]table2_upper!$B5</f>
+      <c r="D6" s="5">
+        <f>[12]table2_upper!$B5</f>
         <v>1.85</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7">
-        <f>[12]table2!C5</f>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5">
+        <f>[11]table2!C5</f>
         <v>3.41</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="5">
         <f>[10]table2_lower!C5</f>
         <v>1.8</v>
       </c>
-      <c r="H6" s="7">
-        <f>[11]table2_upper!$C5</f>
+      <c r="H6" s="5">
+        <f>[12]table2_upper!$C5</f>
         <v>5.32</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7">
-        <f>[12]table2!D5</f>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5">
+        <f>[11]table2!D5</f>
         <v>4.07</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="5">
         <f>[10]table2_lower!D5</f>
-        <v>2.54</v>
-      </c>
-      <c r="L6" s="7">
-        <f>[11]table2_upper!$D5</f>
-        <v>5.74</v>
+        <v>2.41</v>
+      </c>
+      <c r="L6" s="5">
+        <f>[12]table2_upper!$D5</f>
+        <v>5.91</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="7">
-        <f>[12]table2!B6</f>
+      <c r="B7" s="5">
+        <f>[11]table2!B6</f>
         <v>4.2699999999999996</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <f>[10]table2_lower!B6</f>
         <v>3.17</v>
       </c>
-      <c r="D7" s="7">
-        <f>[11]table2_upper!$B6</f>
+      <c r="D7" s="5">
+        <f>[12]table2_upper!$B6</f>
         <v>5.55</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7">
-        <f>[12]table2!C6</f>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <f>[11]table2!C6</f>
         <v>10.24</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G7" s="5">
         <f>[10]table2_lower!C6</f>
         <v>5.4</v>
       </c>
-      <c r="H7" s="7">
-        <f>[11]table2_upper!$C6</f>
+      <c r="H7" s="5">
+        <f>[12]table2_upper!$C6</f>
         <v>15.95</v>
       </c>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7">
-        <f>[12]table2!D6</f>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5">
+        <f>[11]table2!D6</f>
         <v>12.2</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K7" s="5">
         <f>[10]table2_lower!D6</f>
-        <v>7.63</v>
-      </c>
-      <c r="L7" s="7">
-        <f>[11]table2_upper!$D6</f>
-        <v>17.21</v>
+        <v>7.23</v>
+      </c>
+      <c r="L7" s="5">
+        <f>[12]table2_upper!$D6</f>
+        <v>17.73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>